<commit_message>
23.1. Meeting fixed Boundary Condition
</commit_message>
<xml_diff>
--- a/Balken/Kragarm Benchmark.xlsx
+++ b/Balken/Kragarm Benchmark.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC817304-C12A-4250-8338-6EDEE2F61DFB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E110A0-2157-44D7-8C44-E0095D4055EB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Lambda</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t>lam*PL²/EI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l²/EI </t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -367,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D13"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,7 +391,7 @@
     <col min="4" max="4" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -389,8 +401,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -401,8 +416,12 @@
         <f>B3*B4*B2^2/(B5*B6)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <f>H5^2/H6/H7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -410,15 +429,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <v>210000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -426,8 +451,14 @@
         <f>B2^2 /B5</f>
         <v>4.761904761904762E-9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -435,8 +466,14 @@
         <f>(B6*12)^(1/4)</f>
         <v>1.5461103513878914E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -445,7 +482,7 @@
         <v>2.3904572186687889E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>29684</v>
       </c>

</xml_diff>